<commit_message>
added metrics, fixed minimum fitness metric
</commit_message>
<xml_diff>
--- a/simulations/synthetic_data_20.xlsx
+++ b/simulations/synthetic_data_20.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,21 +476,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sec A, Sec B, Sec C</t>
+          <t>Sec A</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>XXAB</t>
+          <t>XXEG</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Prof AM, Prof V, Prof P, Prof Y</t>
+          <t>Prof I</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -501,21 +501,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sec D, Sec E, Sec F</t>
+          <t>Sec A</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>XXZ</t>
+          <t>XXL</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Prof AD</t>
+          <t>Prof P</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -526,17 +526,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sec G, Sec H, Sec I</t>
+          <t>Sec A</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>XXAO</t>
+          <t>XXER</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Prof R</t>
+          <t>Prof CG</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -551,21 +551,21 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sec J, Sec K, Sec L</t>
+          <t>Sec A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>XXBO</t>
+          <t>XXAO</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Prof AM, Prof Z, Prof H, Prof B</t>
+          <t>Prof CF</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -576,17 +576,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sec M, Sec N, Sec O</t>
+          <t>Sec A</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>XXAU</t>
+          <t>XXDK</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Prof J, Prof Q, Prof AD</t>
+          <t>Prof L</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -601,23 +601,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sec P, Sec Q, Sec R</t>
+          <t>Sec A</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>XXC</t>
+          <t>XXAV</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Prof V, Prof M, Prof F, Prof J</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>Prof AS, Prof BI, Prof CG, Prof AA</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
       <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -626,23 +626,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec A</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>XXR, XXBJ</t>
+          <t>XXFK</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Prof S, Prof AM</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>Prof BA, Prof CH, Prof CK, Prof BM</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
       <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -651,21 +651,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec B</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>XXAV</t>
+          <t>XXEU</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Prof AB, Prof T</t>
+          <t>Prof Q</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
@@ -676,17 +676,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sec J</t>
+          <t>Sec B</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>XXAN, XXB</t>
+          <t>XXEA</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Prof AG, Prof N</t>
+          <t>Prof BU</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -701,21 +701,21 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sec R</t>
+          <t>Sec B</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>XXBJ</t>
+          <t>XXAS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Prof AL, Prof D, Prof Z</t>
+          <t>Prof AW</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
@@ -726,17 +726,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec B</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>XXE, XXAZ</t>
+          <t>XXDY</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Prof L, Prof AD</t>
+          <t>Prof AD</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -751,21 +751,21 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sec I</t>
+          <t>Sec B</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>XXH, XXAE</t>
+          <t>XXCT</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Prof AN, Prof F, Prof AH, Prof Y</t>
+          <t>Prof CD</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -781,18 +781,18 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>XXAK, XXW</t>
+          <t>XXG</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Prof AK, Prof F, Prof B, Prof V</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>2</v>
-      </c>
-      <c r="F14" t="inlineStr"/>
+          <t>Prof CS, Prof AR, Prof AW, Prof BI</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
       <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
@@ -801,23 +801,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sec M</t>
+          <t>Sec B</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>XXA, XXK</t>
+          <t>XXCN</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Prof AE, Prof S</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
+          <t>Prof AR, Prof BY, Prof CH, Prof AN</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
       <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -826,21 +826,21 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sec F</t>
+          <t>Sec C</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>XXAY, XXE</t>
+          <t>XXDC</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Prof W, Prof E, Prof C, Prof AK</t>
+          <t>Prof C</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
@@ -851,17 +851,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sec A</t>
+          <t>Sec C</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>XXAV</t>
+          <t>XXAF</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Prof P, Prof T, Prof R, Prof Q</t>
+          <t>Prof DB</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -876,21 +876,21 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sec E</t>
+          <t>Sec C</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>XXH</t>
+          <t>XXCG</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Prof X, Prof M, Prof Q</t>
+          <t>Prof AH</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
@@ -906,12 +906,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>XXN, XXAK</t>
+          <t>XXBP</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Prof X, Prof F</t>
+          <t>Prof AV</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -926,17 +926,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sec L</t>
+          <t>Sec C</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>XXBH, XXBJ</t>
+          <t>XXDG</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Prof AG, Prof C, Prof AE</t>
+          <t>Prof BN</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -951,23 +951,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sec E</t>
+          <t>Sec C</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>XXBN</t>
+          <t>XXAG</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Prof U, Prof V, Prof I</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>3</v>
-      </c>
-      <c r="F21" t="inlineStr"/>
+          <t>Prof AD, Prof L, Prof T, Prof AI</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>2</v>
+      </c>
       <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -976,23 +976,23 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sec B</t>
+          <t>Sec C</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>XXV</t>
+          <t>XXS</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Prof AG</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>4</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
+          <t>Prof BW, Prof CQ, Prof AL, Prof AY</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>2</v>
+      </c>
       <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
@@ -1001,23 +1001,23 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sec M</t>
+          <t>Sec D</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>XXH, XXW</t>
+          <t>XXEX</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Prof I, Prof A, Prof H</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof BV</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>4</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
     </row>
     <row r="24">
@@ -1026,23 +1026,23 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Sec B</t>
+          <t>Sec D</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>XXU</t>
+          <t>XXI</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Prof Z, Prof AA</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof BX</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
@@ -1051,21 +1051,21 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sec O</t>
+          <t>Sec D</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>XXEO</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Prof I, Prof J</t>
+          <t>Prof CM</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
@@ -1076,17 +1076,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sec R</t>
+          <t>Sec D</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>XXBK, XXV</t>
+          <t>XXDQ</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Prof AM, Prof T, Prof K</t>
+          <t>Prof E</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1101,17 +1101,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sec L</t>
+          <t>Sec D</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>XXAQ</t>
+          <t>XXCQ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Prof AK</t>
+          <t>Prof DD</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1126,23 +1126,23 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec D</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>XXK</t>
+          <t>XXFM</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Prof K, Prof AL</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>2</v>
-      </c>
-      <c r="F28" t="inlineStr"/>
+          <t>Prof CD, Prof AM, Prof AT, Prof AH</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
       <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
@@ -1151,23 +1151,23 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sec I</t>
+          <t>Sec D</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>XXS</t>
+          <t>XXDB</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Prof AB, Prof Q, Prof E, Prof C</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
-        <v>3</v>
-      </c>
-      <c r="F29" t="inlineStr"/>
+          <t>Prof AL, Prof BP, Prof CQ, Prof BX</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
       <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
@@ -1176,21 +1176,21 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Sec B</t>
+          <t>Sec E</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>XXD</t>
+          <t>XXDM</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Prof AF, Prof AG, Prof AD, Prof Z</t>
+          <t>Prof BD</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
@@ -1201,23 +1201,23 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sec D</t>
+          <t>Sec E</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>XXS</t>
+          <t>XXEF</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Prof AL, Prof E, Prof AN, Prof AG</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof CI</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>3</v>
+      </c>
+      <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
@@ -1231,16 +1231,16 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>XXAV</t>
+          <t>XXDS</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Prof AH, Prof W, Prof P</t>
+          <t>Prof CF</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -1251,21 +1251,21 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Sec C</t>
+          <t>Sec E</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>XXBC</t>
+          <t>XXX</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Prof AE, Prof B, Prof AC, Prof AG</t>
+          <t>Prof BK</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
@@ -1276,23 +1276,23 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sec R</t>
+          <t>Sec E</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>XXW</t>
+          <t>XXCD</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Prof J, Prof C</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof CO</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>4</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
     </row>
     <row r="35">
@@ -1301,23 +1301,23 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Sec O</t>
+          <t>Sec E</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>XXAQ, XXBI</t>
+          <t>XXCX</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Prof E, Prof W, Prof K</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
-        <v>3</v>
-      </c>
-      <c r="F35" t="inlineStr"/>
+          <t>Prof T, Prof N, Prof AH, Prof AY</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>2</v>
+      </c>
       <c r="G35" t="inlineStr"/>
     </row>
     <row r="36">
@@ -1326,23 +1326,23 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Sec N</t>
+          <t>Sec E</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>XXAD</t>
+          <t>XXCP</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Prof H, Prof O, Prof Z, Prof D</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
-        <v>4</v>
-      </c>
-      <c r="F36" t="inlineStr"/>
+          <t>Prof Y, Prof BA, Prof G, Prof C</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
       <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
@@ -1351,21 +1351,21 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sec C</t>
+          <t>Sec F</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>XXAD, XXS</t>
+          <t>XXDH</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Prof R, Prof K</t>
+          <t>Prof U</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
@@ -1376,21 +1376,21 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sec K</t>
+          <t>Sec F</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>XXN</t>
+          <t>XXAQ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Prof S</t>
+          <t>Prof BB</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
@@ -1401,17 +1401,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Sec C</t>
+          <t>Sec F</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>XXBH</t>
+          <t>XXAZ</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Prof N, Prof AO, Prof D, Prof AK</t>
+          <t>Prof AG</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1426,17 +1426,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Sec D</t>
+          <t>Sec F</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>XXL, XXBP</t>
+          <t>XXEE</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Prof M, Prof X</t>
+          <t>Prof AX</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1451,23 +1451,23 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Sec B</t>
+          <t>Sec F</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>XXAL</t>
+          <t>XXCH</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Prof X</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof AZ</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>4</v>
+      </c>
+      <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
@@ -1476,23 +1476,23 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sec O</t>
+          <t>Sec F</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>XXBP</t>
+          <t>XXDL</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Prof AD, Prof A</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>4</v>
-      </c>
-      <c r="F42" t="inlineStr"/>
+          <t>Prof AX, Prof CJ, Prof DB, Prof AW</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>2</v>
+      </c>
       <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
@@ -1501,17 +1501,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Sec H</t>
+          <t>Sec F</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>XXR</t>
+          <t>XXCO</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Prof AK</t>
+          <t>Prof DA, Prof CY, Prof BV, Prof AG</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -1526,21 +1526,21 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec G</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>XXBI, XXAP</t>
+          <t>XXAU</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Prof P, Prof AN</t>
+          <t>Prof BE</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
@@ -1551,21 +1551,21 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec G</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>XXR</t>
+          <t>XXBM</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Prof AL, Prof Y</t>
+          <t>Prof V</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
@@ -1576,17 +1576,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Sec S</t>
+          <t>Sec G</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>XXBG, XXN</t>
+          <t>XXDI</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Prof X</t>
+          <t>Prof N</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1601,17 +1601,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec G</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>XXU</t>
+          <t>XXCE</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Prof T</t>
+          <t>Prof BK</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1626,21 +1626,21 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Sec T</t>
+          <t>Sec G</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>XXBC, XXAL</t>
+          <t>XXEB</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Prof Q, Prof AN</t>
+          <t>Prof BH</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
@@ -1651,17 +1651,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Sec O</t>
+          <t>Sec G</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>XXI</t>
+          <t>XXBI</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Prof V, Prof C</t>
+          <t>Prof BN, Prof AN, Prof BD, Prof I</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -1676,23 +1676,23 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Sec A</t>
+          <t>Sec G</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>XXAE, XXT</t>
+          <t>XXK</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Prof AO</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>2</v>
-      </c>
-      <c r="F50" t="inlineStr"/>
+          <t>Prof AK, Prof AP, Prof W, Prof CA</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="n">
+        <v>2</v>
+      </c>
       <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
@@ -1701,23 +1701,23 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sec B</t>
+          <t>Sec H</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>XXBJ</t>
+          <t>XXAC</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Prof B, Prof AH</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof CE</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>4</v>
+      </c>
+      <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
     </row>
     <row r="52">
@@ -1726,21 +1726,21 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Sec A</t>
+          <t>Sec H</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>XXAS, XXAD</t>
+          <t>XXCU</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Prof P</t>
+          <t>Prof CK</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
@@ -1756,16 +1756,16 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>XXAN</t>
+          <t>XXFL</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Prof W</t>
+          <t>Prof CM</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
@@ -1776,21 +1776,21 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Sec G</t>
+          <t>Sec H</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>XXAR, XXBP</t>
+          <t>XXFF</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Prof B, Prof K, Prof G, Prof U</t>
+          <t>Prof CP</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
@@ -1801,17 +1801,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Sec N</t>
+          <t>Sec H</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>XXF</t>
+          <t>XXBV</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Prof AP, Prof R, Prof U</t>
+          <t>Prof AK</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1826,23 +1826,23 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Sec F</t>
+          <t>Sec H</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>XXI</t>
+          <t>XXEW</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Prof X, Prof AN, Prof M</t>
-        </is>
-      </c>
-      <c r="E56" t="n">
-        <v>3</v>
-      </c>
-      <c r="F56" t="inlineStr"/>
+          <t>Prof U, Prof AE, Prof BX, Prof O</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="n">
+        <v>2</v>
+      </c>
       <c r="G56" t="inlineStr"/>
     </row>
     <row r="57">
@@ -1851,23 +1851,23 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec H</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>XXAW</t>
+          <t>XXFI</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Prof AJ, Prof AC, Prof AE, Prof M</t>
-        </is>
-      </c>
-      <c r="E57" t="n">
-        <v>2</v>
-      </c>
-      <c r="F57" t="inlineStr"/>
+          <t>Prof D, Prof CC, Prof I, Prof AE</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="n">
+        <v>2</v>
+      </c>
       <c r="G57" t="inlineStr"/>
     </row>
     <row r="58">
@@ -1881,16 +1881,16 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>XXR</t>
+          <t>XXAX</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Prof AC, Prof U</t>
+          <t>Prof BV</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
@@ -1901,21 +1901,21 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Sec K</t>
+          <t>Sec I</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>XXAJ, XXE</t>
+          <t>XXES</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Prof C</t>
+          <t>Prof CC</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
@@ -1926,17 +1926,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Sec C</t>
+          <t>Sec I</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>XXAM, XXBB</t>
+          <t>XXFH</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Prof H, Prof E, Prof C</t>
+          <t>Prof BM</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -1951,21 +1951,21 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Sec T</t>
+          <t>Sec I</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>XXAV, XXD</t>
+          <t>XXBU</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Prof AE, Prof L</t>
+          <t>Prof CR</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
@@ -1976,21 +1976,21 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sec J</t>
+          <t>Sec I</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>XXAX</t>
+          <t>XXFG</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Prof W, Prof AH</t>
+          <t>Prof Q</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
@@ -2001,23 +2001,23 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Sec K</t>
+          <t>Sec I</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>XXAS</t>
+          <t>XXEC</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Prof Y, Prof F</t>
-        </is>
-      </c>
-      <c r="E63" t="n">
-        <v>2</v>
-      </c>
-      <c r="F63" t="inlineStr"/>
+          <t>Prof BY, Prof DA, Prof BB, Prof B</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>2</v>
+      </c>
       <c r="G63" t="inlineStr"/>
     </row>
     <row r="64">
@@ -2026,17 +2026,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec I</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>XXR, XXAV</t>
+          <t>XXP</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Prof P, Prof J, Prof X</t>
+          <t>Prof AU, Prof AG, Prof BH, Prof BQ</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -2051,21 +2051,21 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Sec O</t>
+          <t>Sec J</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>XXAS, XXAN</t>
+          <t>XXB</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Prof AP, Prof B</t>
+          <t>Prof CS</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
@@ -2076,21 +2076,21 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec J</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>XXL</t>
+          <t>XXEM</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Prof F, Prof R</t>
+          <t>Prof BN</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
@@ -2101,23 +2101,23 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Sec F</t>
+          <t>Sec J</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>XXBD, XXBL</t>
+          <t>XXD</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Prof O</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
-      <c r="F67" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof BS</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>3</v>
+      </c>
+      <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
     </row>
     <row r="68">
@@ -2126,21 +2126,21 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Sec G</t>
+          <t>Sec J</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>XXP</t>
+          <t>XXAI</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Prof AA, Prof AF, Prof AJ</t>
+          <t>Prof CE</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
@@ -2151,21 +2151,21 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Sec G</t>
+          <t>Sec J</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>XXJ, XXB</t>
+          <t>XXBJ</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Prof M, Prof I, Prof N, Prof D</t>
+          <t>Prof CZ</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
@@ -2176,23 +2176,23 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Sec M</t>
+          <t>Sec J</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>XXBF</t>
+          <t>XXAA</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Prof AE, Prof Q, Prof Y, Prof AG</t>
-        </is>
-      </c>
-      <c r="E70" t="n">
-        <v>4</v>
-      </c>
-      <c r="F70" t="inlineStr"/>
+          <t>Prof CB, Prof AI, Prof BE, Prof M</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="n">
+        <v>2</v>
+      </c>
       <c r="G70" t="inlineStr"/>
     </row>
     <row r="71">
@@ -2201,23 +2201,23 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Sec I</t>
+          <t>Sec J</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>XXAC</t>
+          <t>XXDR</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Prof O, Prof AL, Prof AG, Prof R</t>
-        </is>
-      </c>
-      <c r="E71" t="n">
-        <v>3</v>
-      </c>
-      <c r="F71" t="inlineStr"/>
+          <t>Prof CK, Prof CX, Prof S, Prof BN</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="n">
+        <v>2</v>
+      </c>
       <c r="G71" t="inlineStr"/>
     </row>
     <row r="72">
@@ -2226,21 +2226,21 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Sec H</t>
+          <t>Sec K</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>XXA, XXAN</t>
+          <t>XXBR</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Prof Y</t>
+          <t>Prof BS</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
@@ -2251,21 +2251,21 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Sec M</t>
+          <t>Sec K</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>XXS</t>
+          <t>XXAL</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Prof AB, Prof AO, Prof H</t>
+          <t>Prof E</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
@@ -2276,17 +2276,17 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Sec S</t>
+          <t>Sec K</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>XXL, XXBE</t>
+          <t>XXFA</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Prof AB</t>
+          <t>Prof DF</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -2301,21 +2301,21 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Sec R</t>
+          <t>Sec K</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>XXAD</t>
+          <t>XXCV</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Prof AG, Prof AK</t>
+          <t>Prof CS</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
@@ -2326,23 +2326,23 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Sec E</t>
+          <t>Sec K</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>XXR, XXN</t>
+          <t>XXO</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Prof AA, Prof O, Prof W, Prof T</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr"/>
-      <c r="F76" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof AL</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>4</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
     </row>
     <row r="77">
@@ -2351,23 +2351,23 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Sec D</t>
+          <t>Sec K</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>XXAP, XXAF</t>
+          <t>XXED</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Prof W, Prof K</t>
-        </is>
-      </c>
-      <c r="E77" t="n">
-        <v>3</v>
-      </c>
-      <c r="F77" t="inlineStr"/>
+          <t>Prof AN, Prof BI, Prof CV, Prof O</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="n">
+        <v>2</v>
+      </c>
       <c r="G77" t="inlineStr"/>
     </row>
     <row r="78">
@@ -2376,23 +2376,23 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Sec J</t>
+          <t>Sec K</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>XXCC</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Prof L, Prof V</t>
-        </is>
-      </c>
-      <c r="E78" t="n">
-        <v>2</v>
-      </c>
-      <c r="F78" t="inlineStr"/>
+          <t>Prof U, Prof CP, Prof DA, Prof D</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="n">
+        <v>2</v>
+      </c>
       <c r="G78" t="inlineStr"/>
     </row>
     <row r="79">
@@ -2401,17 +2401,17 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Sec G</t>
+          <t>Sec L</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>XXT, XXBH</t>
+          <t>XXEQ</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Prof AO, Prof T, Prof P</t>
+          <t>Prof X</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2426,21 +2426,21 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Sec I</t>
+          <t>Sec L</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>XXT</t>
+          <t>XXFN</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Prof AJ, Prof AF</t>
+          <t>Prof DF</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
@@ -2451,21 +2451,21 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Sec B</t>
+          <t>Sec L</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>XXR, XXN</t>
+          <t>XXDE</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Prof AM, Prof AF, Prof K</t>
+          <t>Prof E</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
@@ -2476,23 +2476,23 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Sec D</t>
+          <t>Sec L</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>XXT</t>
+          <t>XXDX</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Prof AE, Prof X, Prof AA, Prof B</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr"/>
-      <c r="F82" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof AM</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>4</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
     </row>
     <row r="83">
@@ -2501,21 +2501,21 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Sec O</t>
+          <t>Sec L</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>XXV</t>
+          <t>XXDT</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Prof C, Prof AB, Prof AH, Prof R</t>
+          <t>Prof BT</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
@@ -2526,23 +2526,23 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec L</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>XXD</t>
+          <t>XXT</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Prof AN, Prof AG, Prof AJ, Prof O</t>
-        </is>
-      </c>
-      <c r="E84" t="n">
-        <v>3</v>
-      </c>
-      <c r="F84" t="inlineStr"/>
+          <t>Prof CI, Prof CB, Prof DB, Prof H</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="n">
+        <v>2</v>
+      </c>
       <c r="G84" t="inlineStr"/>
     </row>
     <row r="85">
@@ -2551,23 +2551,23 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Sec K</t>
+          <t>Sec L</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>XXAL, XXT</t>
+          <t>XXN</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Prof AE, Prof E, Prof R</t>
-        </is>
-      </c>
-      <c r="E85" t="n">
-        <v>2</v>
-      </c>
-      <c r="F85" t="inlineStr"/>
+          <t>Prof Z, Prof AY, Prof G, Prof BX</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="n">
+        <v>2</v>
+      </c>
       <c r="G85" t="inlineStr"/>
     </row>
     <row r="86">
@@ -2576,21 +2576,21 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec M</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>XXI</t>
+          <t>XXEH</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Prof J</t>
+          <t>Prof AT</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
@@ -2601,21 +2601,21 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Sec G</t>
+          <t>Sec M</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>XXO, XXAY</t>
+          <t>XXBZ</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Prof AM</t>
+          <t>Prof G</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
@@ -2626,17 +2626,17 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Sec F</t>
+          <t>Sec M</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>XXS, XXA</t>
+          <t>XXBS</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Prof AO, Prof AG, Prof R, Prof AH</t>
+          <t>Prof CJ</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -2651,17 +2651,17 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Sec I</t>
+          <t>Sec M</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>XXAH, XXAT</t>
+          <t>XXBA</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Prof L, Prof AP</t>
+          <t>Prof CQ</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -2676,23 +2676,23 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Sec D</t>
+          <t>Sec M</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>XXAF, XXBC</t>
+          <t>XXFD</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Prof W</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr"/>
-      <c r="F90" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof BL</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>4</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr"/>
     </row>
     <row r="91">
@@ -2701,23 +2701,23 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Sec K</t>
+          <t>Sec M</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>XXY</t>
+          <t>XXBL</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Prof AM, Prof M, Prof T, Prof C</t>
-        </is>
-      </c>
-      <c r="E91" t="n">
-        <v>4</v>
-      </c>
-      <c r="F91" t="inlineStr"/>
+          <t>Prof AT, Prof O, Prof BJ, Prof D</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr"/>
+      <c r="F91" t="n">
+        <v>2</v>
+      </c>
       <c r="G91" t="inlineStr"/>
     </row>
     <row r="92">
@@ -2726,17 +2726,17 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Sec H</t>
+          <t>Sec M</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>XXY</t>
+          <t>XXBN</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Prof AC, Prof AL</t>
+          <t>Prof CC, Prof R, Prof P, Prof CU</t>
         </is>
       </c>
       <c r="E92" t="inlineStr"/>
@@ -2751,17 +2751,17 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Sec J</t>
+          <t>Sec N</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>XXBB, XXT</t>
+          <t>XXV</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Prof V, Prof S</t>
+          <t>Prof CD</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -2776,21 +2776,21 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Sec F</t>
+          <t>Sec N</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>XXBN, XXAP</t>
+          <t>XXBB</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Prof A</t>
+          <t>Prof L</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr"/>
@@ -2801,23 +2801,23 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Sec C</t>
+          <t>Sec N</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>XXM</t>
+          <t>XXCZ</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Prof AP</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof BC</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>4</v>
+      </c>
+      <c r="F95" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
     </row>
     <row r="96">
@@ -2826,21 +2826,21 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec N</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>XXBE</t>
+          <t>XXDF</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Prof T, Prof D, Prof F, Prof N</t>
+          <t>Prof AQ</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr"/>
@@ -2851,21 +2851,21 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec N</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>XXV, XXBM</t>
+          <t>XXAY</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Prof T, Prof AG</t>
+          <t>Prof BJ</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="inlineStr"/>
       <c r="G97" t="inlineStr"/>
@@ -2876,23 +2876,23 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec N</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>XXAP</t>
+          <t>XXDW</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Prof O</t>
-        </is>
-      </c>
-      <c r="E98" t="n">
-        <v>4</v>
-      </c>
-      <c r="F98" t="inlineStr"/>
+          <t>Prof BS, Prof D, Prof AE, Prof Z</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="n">
+        <v>2</v>
+      </c>
       <c r="G98" t="inlineStr"/>
     </row>
     <row r="99">
@@ -2901,23 +2901,23 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Sec E</t>
+          <t>Sec N</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>XXB, XXV</t>
+          <t>XXBX</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Prof Z</t>
-        </is>
-      </c>
-      <c r="E99" t="n">
-        <v>4</v>
-      </c>
-      <c r="F99" t="inlineStr"/>
+          <t>Prof AT, Prof I, Prof AP, Prof CD</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="n">
+        <v>2</v>
+      </c>
       <c r="G99" t="inlineStr"/>
     </row>
     <row r="100">
@@ -2926,21 +2926,21 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Sec R</t>
+          <t>Sec O</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>XXN</t>
+          <t>XXAD</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Prof D, Prof B</t>
+          <t>Prof BO</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr"/>
@@ -2951,21 +2951,21 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Sec K</t>
+          <t>Sec O</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>XXH</t>
+          <t>XXAP</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Prof AK, Prof AF, Prof L, Prof E</t>
+          <t>Prof AF</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
@@ -2976,21 +2976,21 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Sec K</t>
+          <t>Sec O</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>XXAL, XXAR</t>
+          <t>XXBC</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Prof AO, Prof AM</t>
+          <t>Prof T</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr"/>
@@ -3001,21 +3001,21 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Sec E</t>
+          <t>Sec O</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>XXN, XXBE</t>
+          <t>XXBY</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Prof AP, Prof L, Prof H, Prof AI</t>
+          <t>Prof CI</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr"/>
@@ -3026,17 +3026,17 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec O</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>XXK, XXP</t>
+          <t>XXW</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Prof AG, Prof AK, Prof AJ, Prof U</t>
+          <t>Prof M</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -3051,23 +3051,23 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Sec N</t>
+          <t>Sec O</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>XXBH</t>
+          <t>XXAM</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Prof O, Prof AC, Prof C, Prof N</t>
-        </is>
-      </c>
-      <c r="E105" t="n">
-        <v>3</v>
-      </c>
-      <c r="F105" t="inlineStr"/>
+          <t>Prof BO, Prof A, Prof CQ, Prof CE</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="n">
+        <v>2</v>
+      </c>
       <c r="G105" t="inlineStr"/>
     </row>
     <row r="106">
@@ -3076,23 +3076,23 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Sec S</t>
+          <t>Sec O</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>XXAP, XXAS</t>
+          <t>XXBO</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Prof AI</t>
-        </is>
-      </c>
-      <c r="E106" t="n">
-        <v>3</v>
-      </c>
-      <c r="F106" t="inlineStr"/>
+          <t>Prof AX, Prof CR, Prof Q, Prof R</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="n">
+        <v>2</v>
+      </c>
       <c r="G106" t="inlineStr"/>
     </row>
     <row r="107">
@@ -3101,21 +3101,21 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Sec J</t>
+          <t>Sec P</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>XXBJ, XXAE</t>
+          <t>XXDV</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Prof AO, Prof S</t>
+          <t>Prof AW</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F107" t="inlineStr"/>
       <c r="G107" t="inlineStr"/>
@@ -3126,17 +3126,17 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Sec L</t>
+          <t>Sec P</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>XXBF, XXO</t>
+          <t>XXDZ</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Prof W, Prof AM, Prof V</t>
+          <t>Prof BZ</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -3151,21 +3151,21 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Sec E</t>
+          <t>Sec P</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>XXAM, XXAI</t>
+          <t>XXBQ</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Prof B, Prof AO, Prof AM, Prof T</t>
+          <t>Prof BL</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F109" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
@@ -3176,21 +3176,21 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Sec D</t>
+          <t>Sec P</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>XXL</t>
+          <t>XXBF</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Prof Y, Prof P, Prof O</t>
+          <t>Prof AO</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F110" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
@@ -3201,21 +3201,21 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Sec A</t>
+          <t>Sec P</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>XXAQ, XXP</t>
+          <t>XXE</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Prof C, Prof AM</t>
+          <t>Prof J</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
@@ -3226,17 +3226,17 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Sec J</t>
+          <t>Sec P</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>XXBJ, XXV</t>
+          <t>XXA</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Prof J</t>
+          <t>Prof AG, Prof BS, Prof AC, Prof CP</t>
         </is>
       </c>
       <c r="E112" t="inlineStr"/>
@@ -3251,23 +3251,23 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Sec K</t>
+          <t>Sec P</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>XXH</t>
+          <t>XXAN</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Prof AF, Prof AG, Prof R, Prof AH</t>
-        </is>
-      </c>
-      <c r="E113" t="n">
-        <v>2</v>
-      </c>
-      <c r="F113" t="inlineStr"/>
+          <t>Prof BG, Prof CH, Prof DC, Prof CY</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="n">
+        <v>2</v>
+      </c>
       <c r="G113" t="inlineStr"/>
     </row>
     <row r="114">
@@ -3281,16 +3281,16 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>XXBN</t>
+          <t>XXCB</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Prof A, Prof G, Prof AH, Prof Y</t>
+          <t>Prof BH</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F114" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
@@ -3301,17 +3301,17 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Sec K</t>
+          <t>Sec Q</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>XXAL</t>
+          <t>XXAW</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Prof H, Prof AP, Prof T, Prof P</t>
+          <t>Prof AI</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -3331,12 +3331,12 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>XXAF</t>
+          <t>XXCM</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Prof N, Prof J, Prof V, Prof AB</t>
+          <t>Prof BF</t>
         </is>
       </c>
       <c r="E116" t="n">
@@ -3351,17 +3351,17 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Sec J</t>
+          <t>Sec Q</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>XXT</t>
+          <t>XXR</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Prof Q, Prof AD, Prof K</t>
+          <t>Prof CH</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -3376,21 +3376,21 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Sec L</t>
+          <t>Sec Q</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>XXAW</t>
+          <t>XXCL</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Prof AB, Prof K, Prof AL, Prof S</t>
+          <t>Prof AN</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr"/>
@@ -3401,23 +3401,23 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec Q</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>XXBG, XXR</t>
+          <t>XXCF</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Prof K, Prof AO, Prof AG</t>
-        </is>
-      </c>
-      <c r="E119" t="n">
-        <v>3</v>
-      </c>
-      <c r="F119" t="inlineStr"/>
+          <t>Prof DF, Prof K, Prof BO, Prof AD</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr"/>
+      <c r="F119" t="n">
+        <v>2</v>
+      </c>
       <c r="G119" t="inlineStr"/>
     </row>
     <row r="120">
@@ -3426,23 +3426,23 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Sec R</t>
+          <t>Sec Q</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>XXA, XXI</t>
+          <t>XXBE</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Prof B, Prof A, Prof M</t>
-        </is>
-      </c>
-      <c r="E120" t="n">
-        <v>2</v>
-      </c>
-      <c r="F120" t="inlineStr"/>
+          <t>Prof DD, Prof R, Prof BH, Prof CA</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr"/>
+      <c r="F120" t="n">
+        <v>2</v>
+      </c>
       <c r="G120" t="inlineStr"/>
     </row>
     <row r="121">
@@ -3451,17 +3451,17 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Sec N</t>
+          <t>Sec R</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>XXX</t>
+          <t>XXBG</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Prof AN</t>
+          <t>Prof C</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -3476,21 +3476,21 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Sec I</t>
+          <t>Sec R</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>XXBK, XXV</t>
+          <t>XXQ</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Prof P</t>
+          <t>Prof DA</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F122" t="inlineStr"/>
       <c r="G122" t="inlineStr"/>
@@ -3501,17 +3501,17 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec R</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>XXK</t>
+          <t>XXDU</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Prof Q, Prof AG, Prof T, Prof G</t>
+          <t>Prof AI</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -3526,21 +3526,21 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Sec P</t>
+          <t>Sec R</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>XXAM</t>
+          <t>XXEV</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Prof AK</t>
+          <t>Prof AV</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F124" t="inlineStr"/>
       <c r="G124" t="inlineStr"/>
@@ -3551,21 +3551,21 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Sec S</t>
+          <t>Sec R</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>XXU</t>
+          <t>XXET</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Prof Y, Prof C, Prof H, Prof AL</t>
+          <t>Prof CF</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F125" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
@@ -3576,23 +3576,23 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Sec F</t>
+          <t>Sec R</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>XXBN</t>
+          <t>XXBW</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Prof O</t>
-        </is>
-      </c>
-      <c r="E126" t="n">
-        <v>3</v>
-      </c>
-      <c r="F126" t="inlineStr"/>
+          <t>Prof CS, Prof DF, Prof AB, Prof O</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="n">
+        <v>2</v>
+      </c>
       <c r="G126" t="inlineStr"/>
     </row>
     <row r="127">
@@ -3601,23 +3601,23 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Sec A</t>
+          <t>Sec R</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>XXAY</t>
+          <t>XXCS</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Prof AF</t>
-        </is>
-      </c>
-      <c r="E127" t="n">
-        <v>4</v>
-      </c>
-      <c r="F127" t="inlineStr"/>
+          <t>Prof Q, Prof DE, Prof W, Prof BU</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="n">
+        <v>2</v>
+      </c>
       <c r="G127" t="inlineStr"/>
     </row>
     <row r="128">
@@ -3626,21 +3626,21 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Sec T</t>
+          <t>Sec S</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>XXAT, XXAV</t>
+          <t>XXDJ</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Prof P, Prof V, Prof A</t>
+          <t>Prof AE</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F128" t="inlineStr"/>
       <c r="G128" t="inlineStr"/>
@@ -3651,21 +3651,21 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Sec O</t>
+          <t>Sec S</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>XXU</t>
+          <t>XXC</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Prof F, Prof Y</t>
+          <t>Prof DB</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F129" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
@@ -3676,21 +3676,21 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Sec F</t>
+          <t>Sec S</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>XXM, XXBJ</t>
+          <t>XXBD</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Prof P, Prof V, Prof I, Prof O</t>
+          <t>Prof CF</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F130" t="inlineStr"/>
       <c r="G130" t="inlineStr"/>
@@ -3701,21 +3701,21 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec S</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>XXBH, XXAI</t>
+          <t>XXM</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Prof H, Prof AD, Prof AL</t>
+          <t>Prof BY</t>
         </is>
       </c>
       <c r="E131" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F131" t="inlineStr"/>
       <c r="G131" t="inlineStr"/>
@@ -3731,12 +3731,12 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>XXAR, XXO</t>
+          <t>XXEK</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Prof Z, Prof Y, Prof W, Prof V</t>
+          <t>Prof CP</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -3751,23 +3751,23 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Sec Q</t>
+          <t>Sec S</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>XXAE, XXT</t>
+          <t>XXBH</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Prof M, Prof E, Prof AM, Prof J</t>
-        </is>
-      </c>
-      <c r="E133" t="n">
-        <v>4</v>
-      </c>
-      <c r="F133" t="inlineStr"/>
+          <t>Prof X, Prof BJ, Prof CN, Prof CZ</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="n">
+        <v>2</v>
+      </c>
       <c r="G133" t="inlineStr"/>
     </row>
     <row r="134">
@@ -3776,23 +3776,23 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Sec M</t>
+          <t>Sec S</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>XXX, XXAC</t>
+          <t>XXU</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Prof Q, Prof N, Prof U</t>
-        </is>
-      </c>
-      <c r="E134" t="n">
-        <v>4</v>
-      </c>
-      <c r="F134" t="inlineStr"/>
+          <t>Prof BQ, Prof CK, Prof AB, Prof CB</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr"/>
+      <c r="F134" t="n">
+        <v>2</v>
+      </c>
       <c r="G134" t="inlineStr"/>
     </row>
     <row r="135">
@@ -3801,21 +3801,21 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Sec R</t>
+          <t>Sec T</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>XXBB, XXBL</t>
+          <t>XXF</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Prof K, Prof AG, Prof AP</t>
+          <t>Prof BW</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F135" t="inlineStr"/>
       <c r="G135" t="inlineStr"/>
@@ -3826,21 +3826,21 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Sec A</t>
+          <t>Sec T</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>XXAL</t>
+          <t>XXDA</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Prof H</t>
+          <t>Prof BB</t>
         </is>
       </c>
       <c r="E136" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F136" t="inlineStr"/>
       <c r="G136" t="inlineStr"/>
@@ -3851,23 +3851,23 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Sec N</t>
+          <t>Sec T</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>XXBG</t>
+          <t>XXFJ</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Prof AK</t>
-        </is>
-      </c>
-      <c r="E137" t="inlineStr"/>
-      <c r="F137" t="n">
-        <v>2</v>
-      </c>
+          <t>Prof T</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>3</v>
+      </c>
+      <c r="F137" t="inlineStr"/>
       <c r="G137" t="inlineStr"/>
     </row>
     <row r="138">
@@ -3876,21 +3876,21 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Sec N</t>
+          <t>Sec T</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>XXS</t>
+          <t>XXEZ</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Prof C</t>
+          <t>Prof J</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F138" t="inlineStr"/>
       <c r="G138" t="inlineStr"/>
@@ -3901,17 +3901,17 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Sec A</t>
+          <t>Sec T</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>XXAM, XXAN</t>
+          <t>XXBT</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Prof V, Prof I, Prof H, Prof AO</t>
+          <t>Prof G</t>
         </is>
       </c>
       <c r="E139" t="n">
@@ -3926,23 +3926,23 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Sec G</t>
+          <t>Sec T</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>XXBG</t>
+          <t>XXZ</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Prof AD</t>
-        </is>
-      </c>
-      <c r="E140" t="n">
-        <v>4</v>
-      </c>
-      <c r="F140" t="inlineStr"/>
+          <t>Prof BL, Prof AP, Prof BK, Prof CV</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr"/>
+      <c r="F140" t="n">
+        <v>2</v>
+      </c>
       <c r="G140" t="inlineStr"/>
     </row>
     <row r="141">
@@ -3951,23 +3951,23 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Sec N</t>
+          <t>Sec T</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>XXAC, XXX</t>
+          <t>XXY</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Prof B, Prof F, Prof I</t>
-        </is>
-      </c>
-      <c r="E141" t="n">
-        <v>4</v>
-      </c>
-      <c r="F141" t="inlineStr"/>
+          <t>Prof AY, Prof BJ, Prof BC, Prof AD</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="n">
+        <v>2</v>
+      </c>
       <c r="G141" t="inlineStr"/>
     </row>
     <row r="142">
@@ -3976,22 +3976,24 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Sec H, Sec K, Sec M, Sec F, Sec R, Sec E, Sec L, Sec N, Sec S, Sec T</t>
+          <t>Sec G</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>BLOCKED_141</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr"/>
-      <c r="E142" t="inlineStr"/>
+          <t>XXAR</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Prof A</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>2</v>
+      </c>
       <c r="F142" t="inlineStr"/>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>(1, 8), (2, 7), (4, 7), (4, 8)</t>
-        </is>
-      </c>
+      <c r="G142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -3999,22 +4001,24 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Sec O, Sec E, Sec N, Sec P, Sec M, Sec K, Sec R, Sec G, Sec H, Sec D</t>
+          <t>Sec K, Sec B, Sec O</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>BLOCKED_142</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr"/>
-      <c r="E143" t="inlineStr"/>
+          <t>XXAK</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Prof AL, Prof L, Prof DD</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>2</v>
+      </c>
       <c r="F143" t="inlineStr"/>
-      <c r="G143" t="inlineStr">
-        <is>
-          <t>(2, 1), (3, 2), (3, 7), (3, 8)</t>
-        </is>
-      </c>
+      <c r="G143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -4022,20 +4026,366 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Sec R, Sec C, Sec K, Sec M, Sec N, Sec T, Sec O, Sec P, Sec A, Sec Q</t>
+          <t>Sec K, Sec B, Sec O</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>BLOCKED_143</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr"/>
+          <t>XXH</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Prof AO, Prof Z, Prof CC</t>
+        </is>
+      </c>
       <c r="E144" t="inlineStr"/>
-      <c r="F144" t="inlineStr"/>
-      <c r="G144" t="inlineStr">
-        <is>
-          <t>(1, 2), (4, 2), (5, 2), (5, 8)</t>
+      <c r="F144" t="n">
+        <v>2</v>
+      </c>
+      <c r="G144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Sec C, Sec E, Sec D</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>XXEY</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Prof AJ, Prof C, Prof BC</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>2</v>
+      </c>
+      <c r="F145" t="inlineStr"/>
+      <c r="G145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Sec P, Sec A</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>XXJ</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Prof AX, Prof CR</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>3</v>
+      </c>
+      <c r="F146" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Sec T</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>XXDN</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Prof CB</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>3</v>
+      </c>
+      <c r="F147" t="inlineStr"/>
+      <c r="G147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Sec T</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>XXCW</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Prof CM</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr"/>
+      <c r="F148" t="n">
+        <v>2</v>
+      </c>
+      <c r="G148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Sec Q</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>XXEP</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Prof AS</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>4</v>
+      </c>
+      <c r="F149" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Sec Q</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>XXAJ</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Prof AC</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="n">
+        <v>2</v>
+      </c>
+      <c r="G150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Sec J</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>XXAB</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Prof BB</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>2</v>
+      </c>
+      <c r="F151" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Sec I, Sec N, Sec H</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>XXCA</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Prof BU, Prof AM, Prof M</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>2</v>
+      </c>
+      <c r="F152" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Sec F, Sec R</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>XXCI</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Prof M, Prof BO</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>2</v>
+      </c>
+      <c r="F153" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Sec F, Sec R</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>XXEL</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Prof BV, Prof BP</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="n">
+        <v>2</v>
+      </c>
+      <c r="G154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Sec S, Sec M, Sec L</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>XXDD</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Prof AH, Prof CG, Prof U</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>3</v>
+      </c>
+      <c r="F155" t="inlineStr"/>
+      <c r="G155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Sec A, Sec Q, Sec D, Sec P, Sec N, Sec K</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>BLOCKED_155</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr"/>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="inlineStr"/>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>(1, 2), (2, 2), (3, 1), (3, 2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Sec G, Sec H, Sec J, Sec M, Sec C, Sec F</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>BLOCKED_156</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr"/>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="inlineStr"/>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>(1, 7), (5, 1), (5, 2), (5, 8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Sec F, Sec S, Sec T, Sec M, Sec G, Sec K</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>BLOCKED_157</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr"/>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="inlineStr"/>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>(2, 1), (2, 7), (4, 2), (5, 7)</t>
         </is>
       </c>
     </row>

</xml_diff>